<commit_message>
Test de la création d'un formuliare
Site du Tuto
http://www.excel-plus.fr/vba/excodes/creer-formulaire-personnalise/
</commit_message>
<xml_diff>
--- a/Rdv.xlsx
+++ b/Rdv.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Nom</t>
   </si>
@@ -25,6 +25,240 @@
   </si>
   <si>
     <t>Chambre</t>
+  </si>
+  <si>
+    <t>Nom 01</t>
+  </si>
+  <si>
+    <t>Prenom 01</t>
+  </si>
+  <si>
+    <t>Chambre 01</t>
+  </si>
+  <si>
+    <t>Chambre 02</t>
+  </si>
+  <si>
+    <t>Chambre 03</t>
+  </si>
+  <si>
+    <t>Chambre 04</t>
+  </si>
+  <si>
+    <t>Chambre 05</t>
+  </si>
+  <si>
+    <t>Chambre 06</t>
+  </si>
+  <si>
+    <t>Chambre 07</t>
+  </si>
+  <si>
+    <t>Chambre 08</t>
+  </si>
+  <si>
+    <t>Chambre 09</t>
+  </si>
+  <si>
+    <t>Chambre 10</t>
+  </si>
+  <si>
+    <t>Chambre 11</t>
+  </si>
+  <si>
+    <t>Chambre 12</t>
+  </si>
+  <si>
+    <t>Chambre 13</t>
+  </si>
+  <si>
+    <t>Chambre 14</t>
+  </si>
+  <si>
+    <t>Chambre 15</t>
+  </si>
+  <si>
+    <t>Chambre 16</t>
+  </si>
+  <si>
+    <t>Chambre 17</t>
+  </si>
+  <si>
+    <t>Chambre 18</t>
+  </si>
+  <si>
+    <t>Chambre 19</t>
+  </si>
+  <si>
+    <t>Chambre 20</t>
+  </si>
+  <si>
+    <t>Chambre 21</t>
+  </si>
+  <si>
+    <t>Chambre 22</t>
+  </si>
+  <si>
+    <t>Chambre 23</t>
+  </si>
+  <si>
+    <t>Chambre 24</t>
+  </si>
+  <si>
+    <t>Chambre 25</t>
+  </si>
+  <si>
+    <t>Nom 02</t>
+  </si>
+  <si>
+    <t>Prenom 02</t>
+  </si>
+  <si>
+    <t>Nom 03</t>
+  </si>
+  <si>
+    <t>Prenom 03</t>
+  </si>
+  <si>
+    <t>Nom 04</t>
+  </si>
+  <si>
+    <t>Prenom 04</t>
+  </si>
+  <si>
+    <t>Nom 05</t>
+  </si>
+  <si>
+    <t>Prenom 05</t>
+  </si>
+  <si>
+    <t>Nom 06</t>
+  </si>
+  <si>
+    <t>Prenom 06</t>
+  </si>
+  <si>
+    <t>Nom 07</t>
+  </si>
+  <si>
+    <t>Prenom 07</t>
+  </si>
+  <si>
+    <t>Nom 08</t>
+  </si>
+  <si>
+    <t>Prenom 08</t>
+  </si>
+  <si>
+    <t>Nom 09</t>
+  </si>
+  <si>
+    <t>Prenom 09</t>
+  </si>
+  <si>
+    <t>Nom 10</t>
+  </si>
+  <si>
+    <t>Prenom 10</t>
+  </si>
+  <si>
+    <t>Nom 11</t>
+  </si>
+  <si>
+    <t>Prenom 11</t>
+  </si>
+  <si>
+    <t>Nom 12</t>
+  </si>
+  <si>
+    <t>Prenom 12</t>
+  </si>
+  <si>
+    <t>Nom 13</t>
+  </si>
+  <si>
+    <t>Prenom 13</t>
+  </si>
+  <si>
+    <t>Nom 14</t>
+  </si>
+  <si>
+    <t>Prenom 14</t>
+  </si>
+  <si>
+    <t>Nom 15</t>
+  </si>
+  <si>
+    <t>Prenom 15</t>
+  </si>
+  <si>
+    <t>Nom 16</t>
+  </si>
+  <si>
+    <t>Prenom 16</t>
+  </si>
+  <si>
+    <t>Nom 17</t>
+  </si>
+  <si>
+    <t>Prenom 17</t>
+  </si>
+  <si>
+    <t>Nom 18</t>
+  </si>
+  <si>
+    <t>Prenom 18</t>
+  </si>
+  <si>
+    <t>Nom 19</t>
+  </si>
+  <si>
+    <t>Prenom 19</t>
+  </si>
+  <si>
+    <t>Nom 20</t>
+  </si>
+  <si>
+    <t>Prenom 20</t>
+  </si>
+  <si>
+    <t>Nom 21</t>
+  </si>
+  <si>
+    <t>Prenom 21</t>
+  </si>
+  <si>
+    <t>Nom 22</t>
+  </si>
+  <si>
+    <t>Prenom 22</t>
+  </si>
+  <si>
+    <t>Nom 23</t>
+  </si>
+  <si>
+    <t>Prenom 23</t>
+  </si>
+  <si>
+    <t>Nom 24</t>
+  </si>
+  <si>
+    <t>Prenom 24</t>
+  </si>
+  <si>
+    <t>Nom 25</t>
+  </si>
+  <si>
+    <t>Prenom 25</t>
+  </si>
+  <si>
+    <t>Nom 26</t>
+  </si>
+  <si>
+    <t>Prenom 26</t>
+  </si>
+  <si>
+    <t>Chambre 26</t>
   </si>
 </sst>
 </file>
@@ -363,13 +597,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -380,6 +619,292 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>